<commit_message>
finished first round of routing. no drc errors
</commit_message>
<xml_diff>
--- a/dwg/roboCoolerPwrReq.xlsx
+++ b/dwg/roboCoolerPwrReq.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.E+00"/>
@@ -318,6 +318,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -353,6 +370,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -532,7 +566,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>